<commit_message>
New ALL Funded ARCHES Projects version
More investigators
</commit_message>
<xml_diff>
--- a/datasheets/All names.xlsx
+++ b/datasheets/All names.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\ARCHES\Github\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\OSF Academic Collaborations\Github\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B039516F-0BFA-48B6-8D4A-4736D97D03B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0901825B-8D49-4478-9606-DACB905F26A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$357</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$C$358</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="578">
   <si>
     <t>Name</t>
   </si>
@@ -1362,9 +1362,6 @@
     <t>ryanf@uic.edu</t>
   </si>
   <si>
-    <t>Ryan Reich</t>
-  </si>
-  <si>
     <t>Sandhya Pruthi</t>
   </si>
   <si>
@@ -1759,6 +1756,12 @@
   </si>
   <si>
     <t>Joseph Irudayaraj</t>
+  </si>
+  <si>
+    <t>Ryan Riech</t>
+  </si>
+  <si>
+    <t>Fan Lam</t>
   </si>
 </sst>
 </file>
@@ -2134,10 +2137,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D357"/>
+  <dimension ref="A1:D358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2163,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2177,7 +2180,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2202,7 +2205,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2238,14 +2241,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2267,10 +2270,10 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2313,7 +2316,7 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2321,13 +2324,13 @@
         <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2341,7 +2344,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2350,7 +2353,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2380,7 +2383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2431,7 +2434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2772,7 +2775,7 @@
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
@@ -2802,7 +2805,7 @@
         <v>111</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>10</v>
@@ -2814,7 +2817,7 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -2963,7 +2966,7 @@
         <v>138</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>10</v>
@@ -3082,7 +3085,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>157</v>
       </c>
@@ -3093,89 +3096,87 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>159</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>160</v>
-      </c>
+        <v>577</v>
+      </c>
+      <c r="B88" s="2"/>
       <c r="C88" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>159</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C89" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>161</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="C89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>163</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C90" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>165</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="C91" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>165</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>167</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B93" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="C93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>169</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>171</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C94" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C95" t="s">
         <v>10</v>
@@ -3183,10 +3184,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C96" t="s">
         <v>10</v>
@@ -3194,10 +3195,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>177</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="C97" t="s">
         <v>10</v>
@@ -3205,65 +3206,65 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>499</v>
-      </c>
-      <c r="B98" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>498</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>180</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>180</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>182</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="C100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
+      <c r="C101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B101" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>185</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="B102" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C103" t="s">
         <v>10</v>
@@ -3271,10 +3272,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C104" t="s">
         <v>10</v>
@@ -3282,30 +3283,30 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>191</v>
-      </c>
-      <c r="B105" s="3"/>
+        <v>189</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="C105" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>192</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>193</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="B106" s="3"/>
       <c r="C106" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C107" t="s">
         <v>10</v>
@@ -3313,10 +3314,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>196</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="C108" t="s">
         <v>10</v>
@@ -3324,10 +3325,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>198</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="C109" t="s">
         <v>10</v>
@@ -3335,39 +3336,39 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>200</v>
-      </c>
-      <c r="B110" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>199</v>
+      </c>
       <c r="C110" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B111" s="3"/>
       <c r="C111" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>202</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>203</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="B112" s="3"/>
       <c r="C112" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
@@ -3375,10 +3376,10 @@
     </row>
     <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C114" t="s">
         <v>7</v>
@@ -3386,10 +3387,10 @@
     </row>
     <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C115" t="s">
         <v>7</v>
@@ -3397,10 +3398,10 @@
     </row>
     <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C116" t="s">
         <v>7</v>
@@ -3408,70 +3409,70 @@
     </row>
     <row r="117" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>210</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>212</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C117" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>214</v>
       </c>
-      <c r="B118" s="3"/>
-      <c r="C118" t="s">
+      <c r="B119" s="3"/>
+      <c r="C119" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>215</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C119" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
+      <c r="C120" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>218</v>
-      </c>
       <c r="B121" s="3"/>
-      <c r="C121" t="s">
-        <v>27</v>
+      <c r="C121" s="3" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>219</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>220</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="B122" s="3"/>
       <c r="C122" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C123" t="s">
         <v>10</v>
@@ -3479,63 +3480,63 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>223</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>222</v>
       </c>
       <c r="C124" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>225</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="C125" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>225</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>227</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C126" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>229</v>
-      </c>
-      <c r="B127" s="3"/>
       <c r="C127" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>230</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>231</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="B128" s="3"/>
       <c r="C128" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C129" t="s">
         <v>7</v>
@@ -3543,303 +3544,303 @@
     </row>
     <row r="130" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
+        <v>232</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>234</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C130" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>236</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B132" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>238</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C132" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
+        <v>238</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C133" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>240</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B134" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C133" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3" t="s">
+      <c r="B135" s="3"/>
+      <c r="C135" s="3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>243</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C135" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C136" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>576</v>
-      </c>
-      <c r="B137" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C137" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>575</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="C137" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="3" t="s">
+      <c r="C138" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="B138" s="3"/>
-      <c r="C138" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="B139" s="3"/>
       <c r="C139" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="140" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B140" s="3"/>
       <c r="C140" s="3" t="s">
-        <v>447</v>
+        <v>7</v>
       </c>
     </row>
     <row r="141" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B141" s="3"/>
       <c r="C141" s="3" t="s">
-        <v>7</v>
+        <v>446</v>
       </c>
     </row>
     <row r="142" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+      <c r="A142" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>252</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C142" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="3" t="s">
+      <c r="C143" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B143" s="3"/>
-      <c r="C143" s="3" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+      <c r="B144" s="3"/>
+      <c r="C144" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>255</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="C144" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+      <c r="C145" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>257</v>
       </c>
-      <c r="B145" s="3"/>
-      <c r="C145" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="3" t="s">
+      <c r="B146" s="3"/>
+      <c r="C146" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B146" s="3"/>
-      <c r="C146" s="3" t="s">
+      <c r="B147" s="3"/>
+      <c r="C147" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>259</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B148" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C147" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="3" t="s">
-        <v>564</v>
-      </c>
-      <c r="B148" s="3"/>
-      <c r="C148" s="3" t="s">
+      <c r="C148" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>261</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C149" t="s">
+      <c r="A149" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>263</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="C150" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C150" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>265</v>
-      </c>
-      <c r="B151" s="3"/>
-      <c r="C151" t="s">
-        <v>27</v>
+        <v>263</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>266</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>267</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="B152" s="3"/>
       <c r="C152" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C153" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
+        <v>268</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C154" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>270</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C154" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B155" s="3"/>
-      <c r="C155" s="3" t="s">
+      <c r="C155" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B156" s="3"/>
       <c r="C156" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B157" s="3"/>
       <c r="C157" s="3" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>275</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C158" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B158" s="3"/>
+      <c r="C158" s="3" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>277</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="C159" t="s">
         <v>10</v>
@@ -3847,32 +3848,32 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>277</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C160" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>279</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B161" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C160" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="C161" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>281</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="C161" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>283</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="C162" t="s">
         <v>7</v>
@@ -3880,105 +3881,105 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>285</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="C163" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>285</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C164" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>287</v>
       </c>
-      <c r="B164" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C164" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+      <c r="C165" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>289</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C165" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
+      <c r="C166" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>291</v>
       </c>
-      <c r="B166" s="4" t="s">
+      <c r="B167" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C166" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+      <c r="C167" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>293</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C167" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
+      <c r="C168" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B168" s="3"/>
-      <c r="C168" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+      <c r="B169" s="3"/>
+      <c r="C169" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
         <v>296</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="C169" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
+      <c r="C170" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
         <v>298</v>
       </c>
-      <c r="B170" s="3"/>
-      <c r="C170" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="B171" s="3"/>
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
         <v>299</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B172" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="C171" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
-        <v>301</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>302</v>
       </c>
       <c r="C172" t="s">
         <v>7</v>
@@ -3986,224 +3987,224 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
+        <v>301</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C173" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
         <v>303</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B174" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="C173" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="3" t="s">
+      <c r="C174" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B175" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="B174" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
+      <c r="C175" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
         <v>305</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C175" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+      <c r="C176" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
         <v>307</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C176" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
-        <v>309</v>
-      </c>
-      <c r="B177" s="4" t="s">
-        <v>310</v>
-      </c>
       <c r="C177" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>311</v>
-      </c>
-      <c r="B178" s="3"/>
+        <v>309</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>310</v>
+      </c>
       <c r="C178" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>311</v>
+      </c>
+      <c r="B179" s="3"/>
+      <c r="C179" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
         <v>312</v>
       </c>
-      <c r="B179" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C179" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
-        <v>314</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="C180" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>314</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C181" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
         <v>316</v>
       </c>
-      <c r="B181" s="10" t="s">
+      <c r="B182" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="C181" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="3" t="s">
+      <c r="C182" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
+      <c r="B183" s="3"/>
+      <c r="C183" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
         <v>319</v>
       </c>
-      <c r="B183" s="4" t="s">
+      <c r="B184" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="C183" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
-        <v>321</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="C184" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>321</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C185" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
         <v>323</v>
       </c>
-      <c r="B185" s="4" t="s">
+      <c r="B186" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C185" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+      <c r="C186" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
         <v>325</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B187" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C186" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="3" t="s">
+      <c r="C187" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B187" s="3"/>
-      <c r="C187" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="3" t="s">
+      <c r="B188" s="3"/>
+      <c r="C188" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="C188" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
-        <v>330</v>
-      </c>
-      <c r="B189" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C189" t="s">
+      <c r="C189" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>330</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C190" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
         <v>332</v>
       </c>
-      <c r="B190" s="4" t="s">
+      <c r="B191" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C190" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+      <c r="C191" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
         <v>334</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B192" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C191" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
-        <v>336</v>
-      </c>
-      <c r="B192" s="4" t="s">
-        <v>337</v>
-      </c>
       <c r="C192" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C193" t="s">
         <v>10</v>
@@ -4211,76 +4212,76 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
+        <v>338</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C194" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
         <v>340</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B195" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C195" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
         <v>342</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B196" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C195" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
-        <v>344</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>345</v>
-      </c>
       <c r="C196" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C197" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C198" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
+        <v>348</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C199" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
         <v>350</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B200" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="C199" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A200" t="s">
-        <v>352</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>353</v>
       </c>
       <c r="C200" t="s">
         <v>7</v>
@@ -4288,252 +4289,255 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>352</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C201" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
         <v>354</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="B202" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C201" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A202" t="s">
-        <v>356</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>357</v>
-      </c>
       <c r="C202" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>358</v>
-      </c>
-      <c r="B203" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>357</v>
       </c>
       <c r="C203" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>360</v>
-      </c>
-      <c r="B204" s="3"/>
+        <v>358</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>359</v>
+      </c>
       <c r="C204" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>360</v>
+      </c>
+      <c r="B205" s="3"/>
+      <c r="C205" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
         <v>361</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B206" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C205" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A206" t="s">
+      <c r="C206" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
         <v>363</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="B207" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C206" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="3" t="s">
+      <c r="C207" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A208" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="B207" s="3"/>
-      <c r="C207" s="3"/>
-    </row>
-    <row r="208" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A208" t="s">
+      <c r="B208" s="3"/>
+      <c r="C208" s="3"/>
+    </row>
+    <row r="209" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
         <v>366</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B209" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C208" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209" t="s">
-        <v>368</v>
-      </c>
-      <c r="B209" s="4" t="s">
-        <v>369</v>
-      </c>
       <c r="C209" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>368</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C210" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
         <v>370</v>
       </c>
-      <c r="B210" s="4" t="s">
+      <c r="B211" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="C210" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A211" t="s">
+      <c r="C211" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
         <v>372</v>
       </c>
-      <c r="B211" s="5" t="s">
+      <c r="B212" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C211" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A212" t="s">
+      <c r="C212" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
         <v>374</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B213" s="4" t="s">
         <v>375</v>
       </c>
-      <c r="C212" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="B213" s="3"/>
-      <c r="C213" s="3" t="s">
-        <v>10</v>
+      <c r="C213" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B214" s="3"/>
       <c r="C214" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A215" t="s">
-        <v>378</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C215" t="s">
-        <v>7</v>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B215" s="3"/>
+      <c r="C215" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
+        <v>378</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C216" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
         <v>380</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="B217" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="C216" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A217" s="3" t="s">
+      <c r="C217" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="B217" s="3"/>
-      <c r="C217" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
+      <c r="B218" s="3"/>
+      <c r="C218" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
         <v>383</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B219" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="C218" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A219" s="3" t="s">
+      <c r="C219" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="B219" s="3"/>
-      <c r="C219" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A220" t="s">
-        <v>386</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C220" t="s">
-        <v>7</v>
+      <c r="B220" s="3"/>
+      <c r="C220" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>388</v>
-      </c>
-      <c r="B221" s="3"/>
+        <v>386</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="C221" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>414</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>389</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="B222" s="3"/>
       <c r="C222" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>575</v>
-      </c>
-      <c r="C223" s="3" t="s">
-        <v>10</v>
+        <v>414</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C223" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>390</v>
-      </c>
-      <c r="B224" t="s">
-        <v>391</v>
-      </c>
-      <c r="C224" t="s">
+        <v>574</v>
+      </c>
+      <c r="C224" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>392</v>
+        <v>390</v>
+      </c>
+      <c r="B225" t="s">
+        <v>391</v>
       </c>
       <c r="C225" t="s">
         <v>10</v>
@@ -4541,10 +4545,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>393</v>
-      </c>
-      <c r="B226" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C226" t="s">
         <v>10</v>
@@ -4552,10 +4553,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B227" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C227" t="s">
         <v>10</v>
@@ -4563,10 +4564,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B228" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C228" t="s">
         <v>10</v>
@@ -4574,15 +4575,18 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>399</v>
-      </c>
-      <c r="C229" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B229" t="s">
+        <v>398</v>
+      </c>
+      <c r="C229" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C230" s="3" t="s">
         <v>10</v>
@@ -4590,7 +4594,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>10</v>
@@ -4598,40 +4602,37 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>402</v>
-      </c>
-      <c r="B232" t="s">
-        <v>403</v>
-      </c>
-      <c r="C232" t="s">
+        <v>401</v>
+      </c>
+      <c r="C232" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>404</v>
-      </c>
-      <c r="C233" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B233" t="s">
+        <v>403</v>
+      </c>
+      <c r="C233" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>405</v>
-      </c>
-      <c r="B234" t="s">
-        <v>406</v>
-      </c>
-      <c r="C234" t="s">
+        <v>404</v>
+      </c>
+      <c r="C234" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B235" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C235" t="s">
         <v>10</v>
@@ -4648,75 +4649,75 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B237" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C237" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>411</v>
+        <v>409</v>
+      </c>
+      <c r="B238" t="s">
+        <v>410</v>
       </c>
       <c r="C238" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
+        <v>411</v>
+      </c>
+      <c r="C239" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
         <v>412</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B240" t="s">
         <v>413</v>
       </c>
-      <c r="C239" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A240" t="s">
+      <c r="C240" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
         <v>414</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B241" t="s">
         <v>415</v>
       </c>
-      <c r="C240" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
+      <c r="C241" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
         <v>416</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B242" t="s">
         <v>417</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C242" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A242" t="s">
-        <v>418</v>
-      </c>
-      <c r="B242" t="s">
-        <v>415</v>
-      </c>
-      <c r="C242" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B243" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C243" t="s">
         <v>7</v>
@@ -4724,73 +4725,73 @@
     </row>
     <row r="244" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
+        <v>419</v>
+      </c>
+      <c r="B244" t="s">
+        <v>420</v>
+      </c>
+      <c r="C244" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
         <v>421</v>
       </c>
-      <c r="B244" t="s">
+      <c r="B245" t="s">
         <v>422</v>
       </c>
-      <c r="C244" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A245" t="s">
-        <v>423</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>424</v>
-      </c>
       <c r="C245" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
+        <v>423</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C246" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
         <v>425</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>426</v>
       </c>
-      <c r="C246" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A247" t="s">
-        <v>427</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>447</v>
+      <c r="C247" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="248" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
+        <v>427</v>
+      </c>
+      <c r="C248" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
         <v>428</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B249" t="s">
         <v>429</v>
       </c>
-      <c r="C248" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A249" t="s">
-        <v>430</v>
-      </c>
-      <c r="B249" t="s">
-        <v>431</v>
-      </c>
       <c r="C249" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B250" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C250" t="s">
         <v>10</v>
@@ -4798,10 +4799,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B251" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C251" t="s">
         <v>10</v>
@@ -4809,10 +4810,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B252" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C252" t="s">
         <v>10</v>
@@ -4820,10 +4821,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B253" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C253" t="s">
         <v>10</v>
@@ -4831,10 +4832,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B254" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C254" t="s">
         <v>10</v>
@@ -4842,54 +4843,54 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
+        <v>440</v>
+      </c>
+      <c r="B255" t="s">
+        <v>441</v>
+      </c>
+      <c r="C255" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
         <v>442</v>
       </c>
-      <c r="B255" s="2" t="s">
+      <c r="B256" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C256" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="256" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A256" t="s">
-        <v>444</v>
-      </c>
-      <c r="B256" t="s">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>576</v>
+      </c>
+      <c r="B257" t="s">
         <v>422</v>
       </c>
-      <c r="C256" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A257" t="s">
-        <v>445</v>
-      </c>
-      <c r="B257" t="s">
-        <v>446</v>
-      </c>
       <c r="C257" t="s">
-        <v>447</v>
+        <v>7</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B258" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C258" t="s">
-        <v>10</v>
+        <v>446</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B259" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C259" t="s">
         <v>10</v>
@@ -4897,10 +4898,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B260" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C260" t="s">
         <v>10</v>
@@ -4908,48 +4909,48 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>454</v>
+        <v>451</v>
+      </c>
+      <c r="B261" t="s">
+        <v>452</v>
       </c>
       <c r="C261" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>455</v>
-      </c>
-      <c r="B262" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C262" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>457</v>
-      </c>
-      <c r="C263" s="3" t="s">
-        <v>447</v>
+        <v>454</v>
+      </c>
+      <c r="B263" t="s">
+        <v>455</v>
+      </c>
+      <c r="C263" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>458</v>
-      </c>
-      <c r="B264" t="s">
-        <v>459</v>
-      </c>
-      <c r="C264" t="s">
-        <v>7</v>
+        <v>456</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B265" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C265" t="s">
         <v>7</v>
@@ -4957,10 +4958,10 @@
     </row>
     <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B266" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C266" t="s">
         <v>7</v>
@@ -4968,10 +4969,10 @@
     </row>
     <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B267" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C267" t="s">
         <v>7</v>
@@ -4979,32 +4980,32 @@
     </row>
     <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
+        <v>463</v>
+      </c>
+      <c r="B268" t="s">
+        <v>464</v>
+      </c>
+      <c r="C268" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>465</v>
+      </c>
+      <c r="B269" t="s">
         <v>466</v>
       </c>
-      <c r="B268" t="s">
-        <v>467</v>
-      </c>
-      <c r="C268" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A269" t="s">
-        <v>468</v>
-      </c>
-      <c r="B269" t="s">
-        <v>469</v>
-      </c>
       <c r="C269" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B270" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C270" t="s">
         <v>10</v>
@@ -5012,264 +5013,264 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
+        <v>469</v>
+      </c>
+      <c r="B271" t="s">
+        <v>470</v>
+      </c>
+      <c r="C271" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>471</v>
+      </c>
+      <c r="B272" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="B271" s="2" t="s">
+      <c r="C272" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
         <v>473</v>
       </c>
-      <c r="C271" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A272" t="s">
+      <c r="B273" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B272" s="2" t="s">
+      <c r="C273" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
         <v>475</v>
       </c>
-      <c r="C272" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A273" t="s">
-        <v>476</v>
-      </c>
-      <c r="C273" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A274" t="s">
-        <v>477</v>
-      </c>
       <c r="C274" t="s">
-        <v>447</v>
+        <v>10</v>
       </c>
     </row>
     <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
+        <v>476</v>
+      </c>
+      <c r="C275" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>477</v>
+      </c>
+      <c r="B276" t="s">
         <v>478</v>
       </c>
-      <c r="B275" t="s">
-        <v>479</v>
-      </c>
-      <c r="C275" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A276" t="s">
-        <v>480</v>
-      </c>
-      <c r="B276" t="s">
-        <v>481</v>
-      </c>
       <c r="C276" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
+        <v>479</v>
+      </c>
+      <c r="B277" t="s">
+        <v>480</v>
+      </c>
+      <c r="C277" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>481</v>
+      </c>
+      <c r="B278" t="s">
         <v>482</v>
       </c>
-      <c r="B277" t="s">
-        <v>483</v>
-      </c>
-      <c r="C277" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A278" t="s">
-        <v>484</v>
-      </c>
-      <c r="B278" s="2" t="s">
-        <v>485</v>
-      </c>
       <c r="C278" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>486</v>
+        <v>483</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>484</v>
       </c>
       <c r="C279" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>487</v>
-      </c>
-      <c r="B280" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C280" t="s">
-        <v>10</v>
+        <v>446</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
+        <v>486</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C281" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>488</v>
+      </c>
+      <c r="B282" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="B281" s="2" t="s">
+      <c r="C282" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
         <v>490</v>
       </c>
-      <c r="C281" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A282" t="s">
+      <c r="B283" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B282" s="2" t="s">
+      <c r="C283" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
         <v>492</v>
       </c>
-      <c r="C282" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A283" t="s">
+      <c r="B284" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B283" s="2" t="s">
+      <c r="C284" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
         <v>494</v>
       </c>
-      <c r="C283" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A284" t="s">
+      <c r="B285" t="s">
+        <v>536</v>
+      </c>
+      <c r="C285" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
         <v>495</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B286" t="s">
         <v>537</v>
       </c>
-      <c r="C284" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A285" t="s">
+      <c r="C286" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
         <v>496</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B287" t="s">
         <v>538</v>
       </c>
-      <c r="C285" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A286" t="s">
-        <v>497</v>
-      </c>
-      <c r="B286" t="s">
-        <v>539</v>
-      </c>
-      <c r="C286" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A287" t="s">
-        <v>498</v>
-      </c>
-      <c r="B287" t="s">
-        <v>540</v>
-      </c>
       <c r="C287" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B288" t="s">
-        <v>179</v>
+        <v>539</v>
       </c>
       <c r="C288" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
+        <v>498</v>
+      </c>
+      <c r="B289" t="s">
+        <v>179</v>
+      </c>
+      <c r="C289" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>499</v>
+      </c>
+      <c r="B290" t="s">
+        <v>540</v>
+      </c>
+      <c r="C290" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
         <v>500</v>
       </c>
-      <c r="B289" t="s">
-        <v>541</v>
-      </c>
-      <c r="C289" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A290" t="s">
-        <v>501</v>
-      </c>
-      <c r="C290" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A291" t="s">
-        <v>502</v>
-      </c>
-      <c r="B291" s="2" t="s">
-        <v>542</v>
-      </c>
       <c r="C291" t="s">
-        <v>10</v>
+        <v>446</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>503</v>
+        <v>501</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>541</v>
       </c>
       <c r="C292" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C293" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C294" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>504</v>
+      </c>
+      <c r="C295" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A295" t="s">
-        <v>506</v>
-      </c>
-      <c r="B295" t="s">
-        <v>543</v>
-      </c>
-      <c r="C295" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="296" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B296" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C296" t="s">
         <v>7</v>
@@ -5277,93 +5278,96 @@
     </row>
     <row r="297" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>508</v>
-      </c>
-      <c r="C297" s="3" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+      <c r="B297" t="s">
+        <v>543</v>
+      </c>
+      <c r="C297" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>509</v>
-      </c>
-      <c r="B298" t="s">
-        <v>545</v>
-      </c>
-      <c r="C298" t="s">
-        <v>10</v>
+        <v>507</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
+        <v>508</v>
+      </c>
+      <c r="B299" t="s">
+        <v>544</v>
+      </c>
+      <c r="C299" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>509</v>
+      </c>
+      <c r="C300" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
         <v>510</v>
       </c>
-      <c r="C299" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A300" t="s">
-        <v>511</v>
-      </c>
-      <c r="C300" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A301" t="s">
-        <v>512</v>
-      </c>
-      <c r="B301" t="s">
-        <v>546</v>
-      </c>
       <c r="C301" t="s">
-        <v>10</v>
+        <v>446</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
+        <v>511</v>
+      </c>
+      <c r="B302" t="s">
+        <v>545</v>
+      </c>
+      <c r="C302" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>512</v>
+      </c>
+      <c r="C303" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
         <v>513</v>
       </c>
-      <c r="C302" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A303" t="s">
+      <c r="C304" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
         <v>514</v>
       </c>
-      <c r="C303" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A304" t="s">
+      <c r="C305" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
         <v>515</v>
-      </c>
-      <c r="C304" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A305" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A306" t="s">
-        <v>517</v>
-      </c>
-      <c r="B306" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="C306" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>518</v>
+        <v>516</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>546</v>
       </c>
       <c r="C307" t="s">
         <v>10</v>
@@ -5371,10 +5375,7 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>519</v>
-      </c>
-      <c r="B308" t="s">
-        <v>548</v>
+        <v>517</v>
       </c>
       <c r="C308" t="s">
         <v>10</v>
@@ -5382,7 +5383,10 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>520</v>
+        <v>518</v>
+      </c>
+      <c r="B309" t="s">
+        <v>547</v>
       </c>
       <c r="C309" t="s">
         <v>10</v>
@@ -5390,43 +5394,40 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
+        <v>519</v>
+      </c>
+      <c r="C310" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>520</v>
+      </c>
+      <c r="B311" t="s">
+        <v>548</v>
+      </c>
+      <c r="C311" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
         <v>521</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B312" t="s">
         <v>549</v>
       </c>
-      <c r="C310" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A311" t="s">
-        <v>522</v>
-      </c>
-      <c r="B311" t="s">
-        <v>550</v>
-      </c>
-      <c r="C311" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A312" t="s">
-        <v>523</v>
-      </c>
-      <c r="B312" t="s">
-        <v>551</v>
-      </c>
       <c r="C312" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B313" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C313" t="s">
         <v>10</v>
@@ -5434,10 +5435,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B314" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C314" t="s">
         <v>10</v>
@@ -5445,26 +5446,26 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>526</v>
+        <v>524</v>
+      </c>
+      <c r="B315" t="s">
+        <v>552</v>
       </c>
       <c r="C315" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C316" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>528</v>
-      </c>
-      <c r="B317" t="s">
-        <v>554</v>
+        <v>526</v>
       </c>
       <c r="C317" t="s">
         <v>10</v>
@@ -5472,7 +5473,10 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>529</v>
+        <v>527</v>
+      </c>
+      <c r="B318" t="s">
+        <v>553</v>
       </c>
       <c r="C318" t="s">
         <v>10</v>
@@ -5480,10 +5484,7 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>530</v>
-      </c>
-      <c r="B319" t="s">
-        <v>555</v>
+        <v>528</v>
       </c>
       <c r="C319" t="s">
         <v>10</v>
@@ -5491,29 +5492,29 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B320" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C320" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>532</v>
+        <v>530</v>
+      </c>
+      <c r="B321" t="s">
+        <v>555</v>
       </c>
       <c r="C321" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>533</v>
-      </c>
-      <c r="B322" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="C322" t="s">
         <v>10</v>
@@ -5521,46 +5522,56 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
+        <v>532</v>
+      </c>
+      <c r="B323" t="s">
+        <v>556</v>
+      </c>
+      <c r="C323" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>533</v>
+      </c>
+      <c r="B324" t="s">
+        <v>557</v>
+      </c>
+      <c r="C324" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
         <v>534</v>
       </c>
-      <c r="B323" t="s">
-        <v>558</v>
-      </c>
-      <c r="C323" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A324" t="s">
-        <v>535</v>
-      </c>
-      <c r="C324" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A325" t="s">
-        <v>536</v>
-      </c>
-      <c r="B325" t="s">
-        <v>559</v>
-      </c>
       <c r="C325" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B326" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C326" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>535</v>
+      </c>
+      <c r="B327" t="s">
+        <v>558</v>
+      </c>
+      <c r="C327" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.3"/>
@@ -5591,8 +5602,9 @@
     <row r="355" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="356" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="357" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="358" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:C357" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:C358" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
         <filter val="UIC"/>
@@ -5662,118 +5674,118 @@
     <hyperlink ref="B85" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
     <hyperlink ref="B86" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
     <hyperlink ref="B87" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B88" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B89" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B90" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B91" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B92" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B93" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B94" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B95" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="B96" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="B97" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="B98" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="B99" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="B100" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="B102" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="B103" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="B104" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="B106" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="B107" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="B108" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="B109" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="B112" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="B113" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="B114" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="B115" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="B116" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="B117" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="B119" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="B122" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="B123" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="B124" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="B125" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="B126" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="B128" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="B129" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="B130" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="B131" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="B132" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="B133" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="B135" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="B136" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="B137" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="B142" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="B144" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="B147" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="B149" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="B150" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="B152" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="B153" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="B154" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="B158" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="B159" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="B160" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="B161" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="B162" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="B163" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="B164" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="B165" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="B166" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="B167" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="B169" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="B171" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="B172" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="B173" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="B175" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="B176" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="B177" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="B179" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="B180" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="B183" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="B184" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="B185" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="B186" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="B189" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="B190" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="B191" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="B192" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="B193" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="B194" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="B195" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="B196" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="B197" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="B198" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="B199" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="B200" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="B201" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="B202" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="B203" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="B205" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="B206" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="B208" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="B209" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="B210" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="B211" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="B212" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="B215" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="B216" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="B218" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="B220" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="B89" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B90" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B91" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B92" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B93" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B94" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B95" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B96" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B97" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="B98" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="B99" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="B100" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="B101" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="B103" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="B104" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="B105" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="B107" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="B108" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="B109" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="B110" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="B113" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="B114" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="B115" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="B116" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="B117" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="B118" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="B120" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="B123" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="B124" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="B125" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="B126" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="B127" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="B129" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="B130" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="B131" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="B132" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="B133" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="B134" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="B136" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="B137" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="B138" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="B143" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="B145" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="B148" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="B150" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="B151" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="B153" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="B154" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="B155" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="B159" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="B160" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="B161" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="B162" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="B163" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="B164" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="B165" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="B166" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="B167" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="B168" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="B170" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="B172" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="B173" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="B174" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="B176" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="B177" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="B178" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="B180" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="B181" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="B184" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="B185" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="B186" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="B187" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="B190" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="B191" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="B192" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="B193" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="B194" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="B195" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="B196" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="B197" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="B198" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="B199" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="B200" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="B201" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="B202" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="B203" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="B204" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="B206" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="B207" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="B209" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="B210" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="B211" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="B212" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="B213" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="B216" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="B217" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="B219" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="B221" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
     <hyperlink ref="B27" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="B222" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="B181" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="B245" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="B255" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="B271" r:id="rId164" display="mailto:siddisu@uic.edu" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="B278" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="B272" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="B280" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="B281" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="B282" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="B283" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="B291" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="B306" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B223" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="B182" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="B246" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="B256" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="B272" r:id="rId164" display="mailto:siddisu@uic.edu" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="B279" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="B273" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="B281" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B282" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B283" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="B284" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B292" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B307" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId173"/>

</xml_diff>